<commit_message>
Spatial FIles HA 2008 - Excel Metadata Files
Spatial FIles HA 2008 - Excel Metadata Files
</commit_message>
<xml_diff>
--- a/Spatial_data/UVic/Harrop-Archibald 2008/Arbutus menziesii Areas/Arbutus menziesii Areas.xlsx
+++ b/Spatial_data/UVic/Harrop-Archibald 2008/Arbutus menziesii Areas/Arbutus menziesii Areas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Documents\GitHub\Github Shackelford-lab\Shackelford-lab\Spatial_data\UVic\Harrop-Archibald 2008\Arbutus menziesii Areas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC5E708-770B-418A-812D-D095C8D1ABFD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08775BB-57B1-42A9-985E-B73199EAC6D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6934027C-8984-4F11-9C55-B9A1F75C2751}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="23700" windowHeight="10785" xr2:uid="{6934027C-8984-4F11-9C55-B9A1F75C2751}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Data table metadata</t>
   </si>
@@ -45,15 +45,9 @@
     <t>Date created</t>
   </si>
   <si>
-    <t>varied</t>
-  </si>
-  <si>
     <t>Date last updated</t>
   </si>
   <si>
-    <t>17-06-2020</t>
-  </si>
-  <si>
     <t>Number of records</t>
   </si>
   <si>
@@ -81,44 +75,81 @@
     <t>Attribute description</t>
   </si>
   <si>
-    <t xml:space="preserve">Batbox on Garry Oak </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arbutus </t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other </t>
-  </si>
-  <si>
-    <t>Ivy</t>
-  </si>
-  <si>
-    <t>Layer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The original layer that the data was gathered from if it was merged. </t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Area where Arbutus menziesii trees were found </t>
-  </si>
-  <si>
     <t>Id</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Identification code of polygons for areas where </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Arbutus menziesii</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> occured.  </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numeric value for each polygon. </t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Site where the area is recorded.</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Values:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">South Woods; Lower Hobbs Cree / Mystic Vale; Haro Woods; Finnerty Ravine. </t>
+    </r>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>22-06-2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +172,13 @@
     </font>
     <font>
       <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -185,11 +223,8 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -212,6 +247,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -529,185 +570,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD12268A-6398-4290-A9FB-F0A6F4DF1282}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="62.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="E9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>